<commit_message>
Updated aerodynamics and validation
High Mach Number Base Pressure method appeared to be giving dodgy results, so commented out to make all shadow flow calculated using Newtonian flow to set Cp = 0. Working much better now, and added inviscid comparison data for all available Mach numbers (from literature)
</commit_message>
<xml_diff>
--- a/AeroPrediction/Validation/VALIDATE1.6.xlsx
+++ b/AeroPrediction/Validation/VALIDATE1.6.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1105531c\Documents\MATLAB\ParticleSwarm\Aura\AeroPrediction\Validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1105531c\Documents\GitHub\High-Speed-Vehicle-Optimisation\AeroPrediction\Validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7590" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Cone-Cylinder" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,46 +752,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-4</c:v>
+                  <c:v>-3.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.99</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.01</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.02</c:v>
+                  <c:v>16.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.02</c:v>
+                  <c:v>20.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.03</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,6 +802,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-0.16089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.3699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.9E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7799999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2326</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45429999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.61460000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9818</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.6606999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.3553999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.0617999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1304,46 +1347,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-4</c:v>
+                  <c:v>-3.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.99</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.01</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.02</c:v>
+                  <c:v>16.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.02</c:v>
+                  <c:v>20.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.03</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,6 +1397,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.1512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15509999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1641</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1673</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16980000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16159999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15479999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1857,40 +1942,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>-4</c:v>
+                  <c:v>-3.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.99</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.01</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.02</c:v>
+                  <c:v>16.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.02</c:v>
+                  <c:v>20.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.03</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.01</c:v>
@@ -1904,6 +1989,45 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.7199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.46E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.21E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.7000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.32E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.3099999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.5199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.5500000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.14810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.49259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.91379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.2424999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.6047</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2401,46 +2525,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-3.99</c:v>
+                  <c:v>-3.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.01</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.01</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.99</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.01</c:v>
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.02</c:v>
+                  <c:v>16.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.010000000000002</c:v>
+                  <c:v>20.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.99</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.020000000000003</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2451,6 +2575,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-0.16089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.3699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.9E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7799999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2326</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45429999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.61460000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9818</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.6606999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.3553999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.0617999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2954,46 +3120,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-3.99</c:v>
+                  <c:v>-3.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.01</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.01</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.99</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.01</c:v>
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.02</c:v>
+                  <c:v>16.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.010000000000002</c:v>
+                  <c:v>20.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.99</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.020000000000003</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3004,6 +3170,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.1512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1484</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15509999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1641</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1673</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16980000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16159999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15479999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3507,46 +3715,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-3.99</c:v>
+                  <c:v>-3.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.01</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.01</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.99</c:v>
+                  <c:v>6.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.01</c:v>
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.02</c:v>
+                  <c:v>16.010000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.010000000000002</c:v>
+                  <c:v>20.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.99</c:v>
+                  <c:v>24.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.020000000000003</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3557,6 +3765,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3.7199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.46E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.21E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.7000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.32E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.3099999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.5199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.5500000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.14810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.49259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.91379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.2424999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.6047</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.9812000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4063,43 +4313,43 @@
                   <c:v>-3.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2</c:v>
+                  <c:v>-1.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.99</c:v>
+                  <c:v>4.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.01</c:v>
+                  <c:v>8.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.01</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.010000000000002</c:v>
+                  <c:v>16.03</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.989999999999998</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>24.02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.03</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4110,6 +4360,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-0.18809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.1800000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8100000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29459999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41349999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5464</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72330000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3499000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1442000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.9062000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6671999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4401000000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4616,43 +4908,43 @@
                   <c:v>-3.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2</c:v>
+                  <c:v>-1.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.99</c:v>
+                  <c:v>4.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.01</c:v>
+                  <c:v>8.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.01</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.010000000000002</c:v>
+                  <c:v>16.03</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.989999999999998</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>24.02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.03</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4663,6 +4955,48 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.18229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20730000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1777</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1255</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1328</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5169,53 +5503,98 @@
                   <c:v>-3.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2</c:v>
+                  <c:v>-1.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.99</c:v>
+                  <c:v>4.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.01</c:v>
+                  <c:v>8.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.01</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.01</c:v>
+                  <c:v>12.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.010000000000002</c:v>
+                  <c:v>16.03</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.989999999999998</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>24.02</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.03</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32</c:v>
+                  <c:v>32.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Circ-Arc-Cylinder-Flare'!$E$3:$E$16</c:f>
+              <c:f>'Circ-Arc-Cylinder-Flare'!$E$3:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5700000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.89E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.3700000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.6300000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1162</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.16600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.24129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.60519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.0552999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.4576</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.8814</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.3167</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2.7473999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9378,6 +9757,9 @@
                 <c:pt idx="13">
                   <c:v>9.4100000000000003E-2</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1056</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9928,6 +10310,45 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5.1700000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.04E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.5699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.5900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.6000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.7300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.12970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.1903</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.44619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.91439999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.3128</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.7130000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -21251,8 +21672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21531,27 +21952,75 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="C17">
+        <v>4.6528</v>
+      </c>
+      <c r="D17">
+        <v>0.1128</v>
+      </c>
+      <c r="E17">
+        <v>-2.6036000000000001</v>
+      </c>
       <c r="G17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>40.020000000000003</v>
+      </c>
+      <c r="C18">
+        <v>5.3071999999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.12529999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-2.9962</v>
+      </c>
       <c r="G18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>44.03</v>
+      </c>
+      <c r="C19">
+        <v>6.1279000000000003</v>
+      </c>
+      <c r="D19">
+        <v>0.12820000000000001</v>
+      </c>
+      <c r="E19">
+        <v>-3.5089000000000001</v>
+      </c>
       <c r="G19">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>48.12</v>
+      </c>
+      <c r="C20">
+        <v>6.7373000000000003</v>
+      </c>
+      <c r="D20">
+        <v>0.14169999999999999</v>
+      </c>
+      <c r="E20">
+        <v>-3.8727999999999998</v>
+      </c>
       <c r="G20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>32</v>
       </c>
@@ -21567,7 +22036,7 @@
   <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21846,27 +22315,75 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>36.020000000000003</v>
+      </c>
+      <c r="C17">
+        <v>5.0358000000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.13170000000000001</v>
+      </c>
+      <c r="E17">
+        <v>-2.6038999999999999</v>
+      </c>
       <c r="G17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>39.99</v>
+      </c>
+      <c r="C18">
+        <v>5.7567000000000004</v>
+      </c>
+      <c r="D18">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-3.0198</v>
+      </c>
       <c r="G18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>6.5077999999999996</v>
+      </c>
+      <c r="D19">
+        <v>0.1628</v>
+      </c>
+      <c r="E19">
+        <v>-3.4590000000000001</v>
+      </c>
       <c r="G19">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>48.01</v>
+      </c>
+      <c r="C20">
+        <v>7.1806999999999999</v>
+      </c>
+      <c r="D20">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="E20">
+        <v>-3.8496000000000001</v>
+      </c>
       <c r="G20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>32</v>
       </c>
@@ -21882,7 +22399,7 @@
   <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21932,6 +22449,9 @@
       <c r="D3">
         <v>0.11840000000000001</v>
       </c>
+      <c r="E3">
+        <v>5.1700000000000003E-2</v>
+      </c>
       <c r="G3">
         <v>-4</v>
       </c>
@@ -21946,6 +22466,9 @@
       <c r="D4">
         <v>0.1163</v>
       </c>
+      <c r="E4">
+        <v>3.3500000000000002E-2</v>
+      </c>
       <c r="G4">
         <v>-2</v>
       </c>
@@ -21959,6 +22482,9 @@
       </c>
       <c r="D5">
         <v>0.1153</v>
+      </c>
+      <c r="E5">
+        <v>1.04E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -21975,6 +22501,9 @@
       <c r="D6">
         <v>0.11600000000000001</v>
       </c>
+      <c r="E6">
+        <v>-1.5699999999999999E-2</v>
+      </c>
       <c r="G6">
         <v>2</v>
       </c>
@@ -21989,6 +22518,9 @@
       <c r="D7">
         <v>0.11840000000000001</v>
       </c>
+      <c r="E7">
+        <v>-3.5900000000000001E-2</v>
+      </c>
       <c r="G7">
         <v>4</v>
       </c>
@@ -22003,6 +22535,9 @@
       <c r="D8">
         <v>0.1215</v>
       </c>
+      <c r="E8">
+        <v>-5.6000000000000001E-2</v>
+      </c>
       <c r="G8">
         <v>6</v>
       </c>
@@ -22017,6 +22552,9 @@
       <c r="D9">
         <v>0.12379999999999999</v>
       </c>
+      <c r="E9">
+        <v>-8.7300000000000003E-2</v>
+      </c>
       <c r="G9">
         <v>8</v>
       </c>
@@ -22031,6 +22569,9 @@
       <c r="D10">
         <v>0.1236</v>
       </c>
+      <c r="E10">
+        <v>-0.12970000000000001</v>
+      </c>
       <c r="G10">
         <v>10</v>
       </c>
@@ -22045,6 +22586,9 @@
       <c r="D11">
         <v>0.1177</v>
       </c>
+      <c r="E11">
+        <v>-0.1903</v>
+      </c>
       <c r="G11">
         <v>12</v>
       </c>
@@ -22059,6 +22603,9 @@
       <c r="D12">
         <v>0.1104</v>
       </c>
+      <c r="E12">
+        <v>-0.44619999999999999</v>
+      </c>
       <c r="G12">
         <v>14</v>
       </c>
@@ -22073,6 +22620,9 @@
       <c r="D13">
         <v>0.10150000000000001</v>
       </c>
+      <c r="E13">
+        <v>-0.91439999999999999</v>
+      </c>
       <c r="G13">
         <v>16</v>
       </c>
@@ -22087,6 +22637,9 @@
       <c r="D14">
         <v>9.5100000000000004E-2</v>
       </c>
+      <c r="E14">
+        <v>-1.3128</v>
+      </c>
       <c r="G14">
         <v>18</v>
       </c>
@@ -22101,6 +22654,9 @@
       <c r="D15">
         <v>8.7099999999999997E-2</v>
       </c>
+      <c r="E15">
+        <v>-1.7130000000000001</v>
+      </c>
       <c r="G15">
         <v>20</v>
       </c>
@@ -22115,31 +22671,82 @@
       <c r="D16">
         <v>9.4100000000000003E-2</v>
       </c>
+      <c r="E16">
+        <v>-2.1257000000000001</v>
+      </c>
       <c r="G16">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>36.020000000000003</v>
+      </c>
+      <c r="C17">
+        <v>4.9455</v>
+      </c>
+      <c r="D17">
+        <v>0.1056</v>
+      </c>
+      <c r="E17">
+        <v>-2.5430999999999999</v>
+      </c>
       <c r="G17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>39.99</v>
+      </c>
+      <c r="C18">
+        <v>5.6765999999999996</v>
+      </c>
+      <c r="D18">
+        <v>0.1202</v>
+      </c>
+      <c r="E18">
+        <v>-2.9550000000000001</v>
+      </c>
       <c r="G18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>43.99</v>
+      </c>
+      <c r="C19">
+        <v>6.3811999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.1356</v>
+      </c>
+      <c r="E19">
+        <v>-3.3645999999999998</v>
+      </c>
       <c r="G19">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>47.99</v>
+      </c>
+      <c r="C20">
+        <v>7.1101999999999999</v>
+      </c>
+      <c r="D20">
+        <v>0.14860000000000001</v>
+      </c>
+      <c r="E20">
+        <v>-3.7924000000000002</v>
+      </c>
       <c r="G20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>32</v>
       </c>
@@ -22154,8 +22761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22197,7 +22804,16 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>-4</v>
+        <v>-3.97</v>
+      </c>
+      <c r="C3">
+        <v>-0.16089999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.1512</v>
+      </c>
+      <c r="E3">
+        <v>3.7199999999999997E-2</v>
       </c>
       <c r="G3">
         <v>-4</v>
@@ -22207,13 +22823,31 @@
       <c r="B4">
         <v>-2</v>
       </c>
+      <c r="C4">
+        <v>-8.3699999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.14929999999999999</v>
+      </c>
+      <c r="E4">
+        <v>2.46E-2</v>
+      </c>
       <c r="G4">
         <v>-2</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>0.02</v>
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="D5">
+        <v>0.1484</v>
+      </c>
+      <c r="E5">
+        <v>1.21E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -22222,7 +22856,16 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>1.99</v>
+        <v>1.98</v>
+      </c>
+      <c r="C6">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.15140000000000001</v>
+      </c>
+      <c r="E6">
+        <v>-2.7000000000000001E-3</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -22230,7 +22873,16 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>4</v>
+        <v>3.99</v>
+      </c>
+      <c r="C7">
+        <v>0.15310000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="E7">
+        <v>-1.32E-2</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -22238,7 +22890,16 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>6.01</v>
+        <v>6.02</v>
+      </c>
+      <c r="C8">
+        <v>0.2326</v>
+      </c>
+      <c r="D8">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="E8">
+        <v>-2.3099999999999999E-2</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -22246,7 +22907,16 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>8</v>
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="C9">
+        <v>0.33169999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.1641</v>
+      </c>
+      <c r="E9">
+        <v>-4.5199999999999997E-2</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -22254,7 +22924,16 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>10</v>
+        <v>10.039999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.45429999999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.1673</v>
+      </c>
+      <c r="E10">
+        <v>-8.5500000000000007E-2</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -22262,7 +22941,16 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>12</v>
+        <v>12.04</v>
+      </c>
+      <c r="C11">
+        <v>0.61460000000000004</v>
+      </c>
+      <c r="D11">
+        <v>0.16980000000000001</v>
+      </c>
+      <c r="E11">
+        <v>-0.14810000000000001</v>
       </c>
       <c r="G11">
         <v>12</v>
@@ -22270,7 +22958,16 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>16.02</v>
+        <v>16.010000000000002</v>
+      </c>
+      <c r="C12">
+        <v>1.2139</v>
+      </c>
+      <c r="D12">
+        <v>0.17030000000000001</v>
+      </c>
+      <c r="E12">
+        <v>-0.49259999999999998</v>
       </c>
       <c r="G12">
         <v>14</v>
@@ -22278,7 +22975,16 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>20.02</v>
+        <v>20.04</v>
+      </c>
+      <c r="C13">
+        <v>1.9818</v>
+      </c>
+      <c r="D13">
+        <v>0.16850000000000001</v>
+      </c>
+      <c r="E13">
+        <v>-0.91379999999999995</v>
       </c>
       <c r="G13">
         <v>16</v>
@@ -22286,7 +22992,16 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>24.03</v>
+        <v>24.01</v>
+      </c>
+      <c r="C14">
+        <v>2.6606999999999998</v>
+      </c>
+      <c r="D14">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="E14">
+        <v>-1.2424999999999999</v>
       </c>
       <c r="G14">
         <v>18</v>
@@ -22296,39 +23011,105 @@
       <c r="B15">
         <v>28.01</v>
       </c>
+      <c r="C15">
+        <v>3.3553999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="E15">
+        <v>-1.6047</v>
+      </c>
       <c r="G15">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>32</v>
+        <v>32.01</v>
+      </c>
+      <c r="C16">
+        <v>4.0617999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="E16">
+        <v>-1.9812000000000001</v>
       </c>
       <c r="G16">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>36.01</v>
+      </c>
+      <c r="C17">
+        <v>4.7676999999999996</v>
+      </c>
+      <c r="D17">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="E17">
+        <v>-2.3687999999999998</v>
+      </c>
       <c r="G17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>39.96</v>
+      </c>
+      <c r="C18">
+        <v>5.4508999999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-2.7498999999999998</v>
+      </c>
       <c r="G18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>44.04</v>
+      </c>
+      <c r="C19">
+        <v>6.1562000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.1812</v>
+      </c>
+      <c r="E19">
+        <v>-3.1524999999999999</v>
+      </c>
       <c r="G19">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>47.99</v>
+      </c>
+      <c r="C20">
+        <v>6.8014000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="E20">
+        <v>-3.5221</v>
+      </c>
       <c r="G20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>32</v>
       </c>
@@ -22341,10 +23122,463 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>-3.97</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.16089999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.1512</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="G3">
+        <v>-4</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-8.3699999999999997E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.14929999999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.46E-2</v>
+      </c>
+      <c r="G4">
+        <v>-2</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.1484</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.21E-2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.15140000000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.15310000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-1.32E-2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>6.02</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.2326</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-2.3099999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.33169999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.1641</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-4.5199999999999997E-2</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.45429999999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.1673</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-8.5500000000000007E-2</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>12.04</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.61460000000000004</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.16980000000000001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-0.14810000000000001</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>16.010000000000002</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.2139</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.17030000000000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-0.49259999999999998</v>
+      </c>
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>20.04</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.9818</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.16850000000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-0.91379999999999995</v>
+      </c>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>24.01</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.6606999999999998</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-1.2424999999999999</v>
+      </c>
+      <c r="G14">
+        <v>18</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>28.01</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3.3553999999999999</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-1.6047</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>32.01</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.0617999999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-1.9812000000000001</v>
+      </c>
+      <c r="G16">
+        <v>22</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>36.01</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4.7676999999999996</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-2.3689</v>
+      </c>
+      <c r="G17">
+        <v>24</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>39.96</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5.4508999999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-2.7498999999999998</v>
+      </c>
+      <c r="G18">
+        <v>26</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>44.04</v>
+      </c>
+      <c r="C19" s="2">
+        <v>6.1562000000000001</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.1812</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-3.1524999999999999</v>
+      </c>
+      <c r="G19">
+        <v>28</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>47.99</v>
+      </c>
+      <c r="C20" s="2">
+        <v>6.8014000000000001</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-3.5221</v>
+      </c>
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:J21"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22388,13 +23622,31 @@
       <c r="B3">
         <v>-3.99</v>
       </c>
+      <c r="C3">
+        <v>-0.18809999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="E3">
+        <v>6.2199999999999998E-2</v>
+      </c>
       <c r="G3">
         <v>-4</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>-2</v>
+        <v>-1.97</v>
+      </c>
+      <c r="C4">
+        <v>-9.1800000000000007E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.20730000000000001</v>
+      </c>
+      <c r="E4">
+        <v>3.5700000000000003E-2</v>
       </c>
       <c r="G4">
         <v>-2</v>
@@ -22402,7 +23654,16 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>-0.01</v>
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>2.3E-3</v>
+      </c>
+      <c r="D5">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="E5">
+        <v>9.4000000000000004E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -22413,6 +23674,15 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6">
+        <v>9.8100000000000007E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="E6">
+        <v>-1.89E-2</v>
+      </c>
       <c r="G6">
         <v>2</v>
       </c>
@@ -22421,194 +23691,14 @@
       <c r="B7">
         <v>4.01</v>
       </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>5.99</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>8.01</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>10.01</v>
-      </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>12</v>
-      </c>
-      <c r="G11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>16.02</v>
-      </c>
-      <c r="G12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>20.010000000000002</v>
-      </c>
-      <c r="G13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>23.99</v>
-      </c>
-      <c r="G14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>28.01</v>
-      </c>
-      <c r="G15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>32.020000000000003</v>
-      </c>
-      <c r="G16">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>-3.99</v>
-      </c>
-      <c r="G3">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>-2</v>
-      </c>
-      <c r="G4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>3.99</v>
+      <c r="C7">
+        <v>0.19009999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.19109999999999999</v>
+      </c>
+      <c r="E7">
+        <v>-4.3700000000000003E-2</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -22618,13 +23708,31 @@
       <c r="B8">
         <v>6.01</v>
       </c>
+      <c r="C8">
+        <v>0.29459999999999997</v>
+      </c>
+      <c r="D8">
+        <v>0.18690000000000001</v>
+      </c>
+      <c r="E8">
+        <v>-7.6300000000000007E-2</v>
+      </c>
       <c r="G8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>8.01</v>
+        <v>8.02</v>
+      </c>
+      <c r="C9">
+        <v>0.41349999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.18260000000000001</v>
+      </c>
+      <c r="E9">
+        <v>-0.1162</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -22632,7 +23740,16 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>10.01</v>
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.5464</v>
+      </c>
+      <c r="D10">
+        <v>0.1777</v>
+      </c>
+      <c r="E10">
+        <v>-0.16600000000000001</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -22640,7 +23757,16 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>12.01</v>
+        <v>12.04</v>
+      </c>
+      <c r="C11">
+        <v>0.72330000000000005</v>
+      </c>
+      <c r="D11">
+        <v>0.17019999999999999</v>
+      </c>
+      <c r="E11">
+        <v>-0.24129999999999999</v>
       </c>
       <c r="G11">
         <v>12</v>
@@ -22648,7 +23774,16 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>16.010000000000002</v>
+        <v>16.03</v>
+      </c>
+      <c r="C12">
+        <v>1.3499000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.1497</v>
+      </c>
+      <c r="E12">
+        <v>-0.60519999999999996</v>
       </c>
       <c r="G12">
         <v>14</v>
@@ -22656,7 +23791,16 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>19.989999999999998</v>
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>2.1442000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.14219999999999999</v>
+      </c>
+      <c r="E13">
+        <v>-1.0552999999999999</v>
       </c>
       <c r="G13">
         <v>16</v>
@@ -22664,7 +23808,16 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>24</v>
+        <v>24.02</v>
+      </c>
+      <c r="C14">
+        <v>2.9062000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.1336</v>
+      </c>
+      <c r="E14">
+        <v>-1.4576</v>
       </c>
       <c r="G14">
         <v>18</v>
@@ -22672,7 +23825,16 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>28.03</v>
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>3.6671999999999998</v>
+      </c>
+      <c r="D15">
+        <v>0.1255</v>
+      </c>
+      <c r="E15">
+        <v>-1.8814</v>
       </c>
       <c r="G15">
         <v>20</v>
@@ -22680,33 +23842,90 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>32</v>
+        <v>32.01</v>
+      </c>
+      <c r="C16">
+        <v>4.4401000000000002</v>
+      </c>
+      <c r="D16">
+        <v>0.1328</v>
+      </c>
+      <c r="E16">
+        <v>-2.3167</v>
       </c>
       <c r="G16">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>36.01</v>
+      </c>
+      <c r="C17">
+        <v>5.1866000000000003</v>
+      </c>
+      <c r="D17">
+        <v>0.1467</v>
+      </c>
+      <c r="E17">
+        <v>-2.7473999999999998</v>
+      </c>
       <c r="G17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>40.03</v>
+      </c>
+      <c r="C18">
+        <v>5.9374000000000002</v>
+      </c>
+      <c r="D18">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E18">
+        <v>-3.1842000000000001</v>
+      </c>
       <c r="G18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>44.02</v>
+      </c>
+      <c r="C19">
+        <v>6.6981000000000002</v>
+      </c>
+      <c r="D19">
+        <v>0.17960000000000001</v>
+      </c>
+      <c r="E19">
+        <v>-3.6392000000000002</v>
+      </c>
       <c r="G19">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>47.98</v>
+      </c>
+      <c r="C20">
+        <v>7.3639000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.19070000000000001</v>
+      </c>
+      <c r="E20">
+        <v>-4.0256999999999996</v>
+      </c>
       <c r="G20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>32</v>
       </c>

</xml_diff>